<commit_message>
Drop down list for sheet name selection added, fail-safe partially implemented on open file, file read
</commit_message>
<xml_diff>
--- a/media/testSet1/SUMMARY OF GSTR-2A_QE DEC'2019.xlsx
+++ b/media/testSet1/SUMMARY OF GSTR-2A_QE DEC'2019.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Py\TallyProject\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Py\TallyProject\media\testSet1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2099" uniqueCount="479">
   <si>
     <t xml:space="preserve">                                           Goods and Services Tax  - GSTR 2A</t>
   </si>
@@ -1495,9 +1495,6 @@
   </si>
   <si>
     <t>S/638/19-20</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
   </si>
   <si>
     <t>ARTEX COMMERCIAL CENTRE</t>
@@ -1678,17 +1675,17 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2070,8 +2067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B205" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A257" workbookViewId="0">
+      <selection activeCell="E275" sqref="E275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2091,82 +2088,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="12" t="s">
@@ -2175,7 +2172,7 @@
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="10" t="s">
         <v>4</v>
       </c>
       <c r="H5" s="13" t="s">
@@ -2193,13 +2190,13 @@
       <c r="L5" s="12"/>
       <c r="M5" s="17"/>
       <c r="N5" s="17"/>
-      <c r="O5" s="8" t="s">
+      <c r="O5" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
@@ -2212,7 +2209,7 @@
       <c r="F6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="11"/>
       <c r="H6" s="14"/>
       <c r="I6" s="16"/>
       <c r="J6" s="14"/>
@@ -2228,7 +2225,7 @@
       <c r="N6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="9"/>
+      <c r="O6" s="11"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -3598,7 +3595,7 @@
         <v>98</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C36" t="s">
         <v>99</v>
@@ -3645,7 +3642,7 @@
         <v>98</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C37" t="s">
         <v>101</v>
@@ -3692,7 +3689,7 @@
         <v>98</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C38" t="s">
         <v>102</v>
@@ -3739,7 +3736,7 @@
         <v>98</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C39" t="s">
         <v>103</v>
@@ -3786,7 +3783,7 @@
         <v>98</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C40" t="s">
         <v>104</v>
@@ -3833,7 +3830,7 @@
         <v>98</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C41" t="s">
         <v>106</v>
@@ -3880,7 +3877,7 @@
         <v>98</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C42" t="s">
         <v>107</v>
@@ -3927,7 +3924,7 @@
         <v>98</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C43" t="s">
         <v>108</v>
@@ -3974,7 +3971,7 @@
         <v>98</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C44" t="s">
         <v>109</v>
@@ -4021,7 +4018,7 @@
         <v>98</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C45" t="s">
         <v>110</v>
@@ -4068,7 +4065,7 @@
         <v>98</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C46" t="s">
         <v>111</v>
@@ -4115,7 +4112,7 @@
         <v>98</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C47" t="s">
         <v>112</v>
@@ -4162,7 +4159,7 @@
         <v>98</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C48" t="s">
         <v>113</v>
@@ -4209,7 +4206,7 @@
         <v>98</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C49" t="s">
         <v>114</v>
@@ -4256,7 +4253,7 @@
         <v>98</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C50" t="s">
         <v>116</v>
@@ -4303,7 +4300,7 @@
         <v>98</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C51" t="s">
         <v>117</v>
@@ -4350,7 +4347,7 @@
         <v>98</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C52" t="s">
         <v>119</v>
@@ -4397,7 +4394,7 @@
         <v>98</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C53" t="s">
         <v>120</v>
@@ -4444,7 +4441,7 @@
         <v>98</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C54" t="s">
         <v>121</v>
@@ -4491,7 +4488,7 @@
         <v>98</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C55" t="s">
         <v>123</v>
@@ -4538,7 +4535,7 @@
         <v>98</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C56" t="s">
         <v>124</v>
@@ -4585,7 +4582,7 @@
         <v>98</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C57" t="s">
         <v>125</v>
@@ -6089,7 +6086,7 @@
         <v>98</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C89" t="s">
         <v>197</v>
@@ -6136,7 +6133,7 @@
         <v>98</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C90" t="s">
         <v>199</v>
@@ -6183,7 +6180,7 @@
         <v>98</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C91" t="s">
         <v>200</v>
@@ -6230,7 +6227,7 @@
         <v>98</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C92" t="s">
         <v>201</v>
@@ -6277,7 +6274,7 @@
         <v>98</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C93" t="s">
         <v>203</v>
@@ -6324,7 +6321,7 @@
         <v>98</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C94" t="s">
         <v>204</v>
@@ -6371,7 +6368,7 @@
         <v>98</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C95" t="s">
         <v>206</v>
@@ -6418,7 +6415,7 @@
         <v>98</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C96" t="s">
         <v>208</v>
@@ -6465,7 +6462,7 @@
         <v>98</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C97" t="s">
         <v>210</v>
@@ -6512,7 +6509,7 @@
         <v>98</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C98" t="s">
         <v>211</v>
@@ -6559,7 +6556,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C99" t="s">
         <v>212</v>
@@ -6606,7 +6603,7 @@
         <v>98</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C100" t="s">
         <v>213</v>
@@ -6653,7 +6650,7 @@
         <v>98</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C101" t="s">
         <v>214</v>
@@ -6700,7 +6697,7 @@
         <v>98</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C102" t="s">
         <v>215</v>
@@ -6747,7 +6744,7 @@
         <v>98</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C103" t="s">
         <v>216</v>
@@ -6794,7 +6791,7 @@
         <v>98</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C104" t="s">
         <v>217</v>
@@ -6841,7 +6838,7 @@
         <v>98</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C105" t="s">
         <v>218</v>
@@ -6888,7 +6885,7 @@
         <v>98</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C106" t="s">
         <v>219</v>
@@ -6935,7 +6932,7 @@
         <v>98</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C107" t="s">
         <v>220</v>
@@ -6982,7 +6979,7 @@
         <v>98</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C108" t="s">
         <v>221</v>
@@ -7029,7 +7026,7 @@
         <v>98</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C109" t="s">
         <v>222</v>
@@ -7076,7 +7073,7 @@
         <v>98</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C110" t="s">
         <v>224</v>
@@ -7123,7 +7120,7 @@
         <v>98</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C111" t="s">
         <v>225</v>
@@ -7170,7 +7167,7 @@
         <v>98</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C112" t="s">
         <v>226</v>
@@ -7217,7 +7214,7 @@
         <v>98</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C113" t="s">
         <v>227</v>
@@ -7264,7 +7261,7 @@
         <v>98</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C114" t="s">
         <v>228</v>
@@ -7311,7 +7308,7 @@
         <v>98</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C115" t="s">
         <v>229</v>
@@ -7358,7 +7355,7 @@
         <v>98</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C116" t="s">
         <v>230</v>
@@ -7405,7 +7402,7 @@
         <v>98</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C117" t="s">
         <v>231</v>
@@ -9144,7 +9141,7 @@
         <v>98</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C154" t="s">
         <v>305</v>
@@ -9191,7 +9188,7 @@
         <v>98</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C155" t="s">
         <v>307</v>
@@ -9238,7 +9235,7 @@
         <v>98</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C156" t="s">
         <v>309</v>
@@ -9285,7 +9282,7 @@
         <v>98</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C157" t="s">
         <v>310</v>
@@ -9332,7 +9329,7 @@
         <v>98</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C158" t="s">
         <v>312</v>
@@ -9379,7 +9376,7 @@
         <v>98</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C159" t="s">
         <v>313</v>
@@ -9426,7 +9423,7 @@
         <v>98</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C160" t="s">
         <v>314</v>
@@ -9473,7 +9470,7 @@
         <v>98</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C161" t="s">
         <v>315</v>
@@ -9520,7 +9517,7 @@
         <v>98</v>
       </c>
       <c r="B162" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C162" t="s">
         <v>316</v>
@@ -9567,7 +9564,7 @@
         <v>98</v>
       </c>
       <c r="B163" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C163" t="s">
         <v>318</v>
@@ -9614,7 +9611,7 @@
         <v>98</v>
       </c>
       <c r="B164" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C164" t="s">
         <v>320</v>
@@ -9661,7 +9658,7 @@
         <v>98</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C165" t="s">
         <v>321</v>
@@ -9708,7 +9705,7 @@
         <v>98</v>
       </c>
       <c r="B166" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C166" t="s">
         <v>323</v>
@@ -9755,7 +9752,7 @@
         <v>98</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C167" t="s">
         <v>325</v>
@@ -9802,7 +9799,7 @@
         <v>98</v>
       </c>
       <c r="B168" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C168" t="s">
         <v>327</v>
@@ -9849,7 +9846,7 @@
         <v>98</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C169" t="s">
         <v>328</v>
@@ -9896,7 +9893,7 @@
         <v>98</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C170" t="s">
         <v>329</v>
@@ -9943,7 +9940,7 @@
         <v>98</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C171" t="s">
         <v>331</v>
@@ -9990,7 +9987,7 @@
         <v>98</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C172" t="s">
         <v>332</v>
@@ -10037,7 +10034,7 @@
         <v>98</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C173" t="s">
         <v>334</v>
@@ -10084,7 +10081,7 @@
         <v>98</v>
       </c>
       <c r="B174" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C174" t="s">
         <v>335</v>
@@ -10131,7 +10128,7 @@
         <v>98</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C175" t="s">
         <v>337</v>
@@ -10178,7 +10175,7 @@
         <v>98</v>
       </c>
       <c r="B176" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C176" t="s">
         <v>338</v>
@@ -10225,7 +10222,7 @@
         <v>98</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C177" t="s">
         <v>340</v>
@@ -10272,7 +10269,7 @@
         <v>98</v>
       </c>
       <c r="B178" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C178" t="s">
         <v>341</v>
@@ -10319,7 +10316,7 @@
         <v>98</v>
       </c>
       <c r="B179" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C179" t="s">
         <v>342</v>
@@ -14451,13 +14448,8 @@
       </c>
     </row>
     <row r="268" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E268" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="F268" s="6">
-        <f>SUBTOTAL(9,F7:F266)</f>
-        <v>4416291.8</v>
-      </c>
+      <c r="E268" s="5"/>
+      <c r="F268" s="6"/>
       <c r="G268" s="6">
         <f>SUBTOTAL(9,G7:G266)</f>
         <v>0</v>
@@ -14467,22 +14459,10 @@
         <v>0</v>
       </c>
       <c r="I268" s="6"/>
-      <c r="J268" s="6">
-        <f>SUBTOTAL(9,J7:J266)</f>
-        <v>3742610.3799999994</v>
-      </c>
-      <c r="K268" s="6">
-        <f>SUBTOTAL(9,K7:K266)</f>
-        <v>40538.79</v>
-      </c>
-      <c r="L268" s="6">
-        <f>SUBTOTAL(9,L7:L266)</f>
-        <v>316566.96999999974</v>
-      </c>
-      <c r="M268" s="6">
-        <f>SUBTOTAL(9,M7:M266)</f>
-        <v>316566.96999999974</v>
-      </c>
+      <c r="J268" s="6"/>
+      <c r="K268" s="6"/>
+      <c r="L268" s="6"/>
+      <c r="M268" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>